<commit_message>
Update Copy of ICD-10 conversions_5_10_20 (3)_JBS.xlsx
</commit_message>
<xml_diff>
--- a/Copy of ICD-10 conversions_5_10_20 (3)_JBS.xlsx
+++ b/Copy of ICD-10 conversions_5_10_20 (3)_JBS.xlsx
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1268" uniqueCount="608">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1281" uniqueCount="610">
   <si>
     <t>Working Number</t>
   </si>
@@ -2561,6 +2561,12 @@
   </si>
   <si>
     <t>I</t>
+  </si>
+  <si>
+    <t>Eligibility</t>
+  </si>
+  <si>
+    <t>Popped--if inclusion for pop it must happen on the same claim</t>
   </si>
 </sst>
 </file>
@@ -3222,7 +3228,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="377">
+  <cellXfs count="379">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4018,16 +4024,6 @@
     <xf numFmtId="0" fontId="0" fillId="38" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4044,9 +4040,6 @@
     <xf numFmtId="0" fontId="0" fillId="37" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4054,16 +4047,10 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="31" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="31" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="31" borderId="0" xfId="0" applyFill="1"/>
@@ -4073,17 +4060,11 @@
     <xf numFmtId="0" fontId="0" fillId="21" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="39" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="39" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
@@ -4093,17 +4074,11 @@
     <xf numFmtId="0" fontId="0" fillId="40" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="41" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="41" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="41" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFill="1"/>
@@ -4113,9 +4088,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="40" fillId="38" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="37" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="40" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="41" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="31" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="39" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -37575,679 +37583,723 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K41"/>
+  <dimension ref="A1:M42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.08203125" defaultRowHeight="15.5"/>
   <cols>
     <col min="2" max="4" width="15.08203125" style="4"/>
-    <col min="5" max="7" width="15.08203125" style="342"/>
-    <col min="8" max="8" width="15.08203125" style="343"/>
-    <col min="9" max="9" width="15.08203125" style="345"/>
-    <col min="10" max="10" width="15.08203125" style="339"/>
+    <col min="5" max="7" width="15.08203125" style="338"/>
+    <col min="8" max="8" width="15.08203125" style="341"/>
+    <col min="9" max="9" width="15.08203125" style="368"/>
+    <col min="13" max="13" width="15.08203125" style="339"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="333"/>
-      <c r="B1" s="341" t="s">
+    <row r="1" spans="1:13">
+      <c r="B1" s="4" t="s">
+        <v>608</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>608</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>608</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>608</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>608</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>608</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>608</v>
+      </c>
+      <c r="I1" s="367" t="s">
+        <v>608</v>
+      </c>
+      <c r="J1" t="s">
+        <v>609</v>
+      </c>
+      <c r="M1" s="4"/>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="333"/>
+      <c r="B2" s="365" t="s">
         <v>594</v>
       </c>
-      <c r="C1" s="341"/>
-      <c r="D1" s="341"/>
-      <c r="E1" s="340" t="s">
+      <c r="C2" s="365"/>
+      <c r="D2" s="365"/>
+      <c r="E2" s="366" t="s">
         <v>597</v>
       </c>
-      <c r="F1" s="340"/>
-      <c r="G1" s="340"/>
-      <c r="H1" s="335"/>
-      <c r="I1" s="344"/>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="334" t="s">
+      <c r="F2" s="366"/>
+      <c r="G2" s="366"/>
+      <c r="H2" s="340"/>
+      <c r="J2" s="365" t="s">
+        <v>594</v>
+      </c>
+      <c r="K2" s="365"/>
+      <c r="L2" s="365"/>
+      <c r="M2" s="335"/>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="334" t="s">
         <v>593</v>
       </c>
-      <c r="B2" s="147" t="s">
+      <c r="B3" s="147" t="s">
         <v>595</v>
       </c>
-      <c r="C2" s="147" t="s">
+      <c r="C3" s="147" t="s">
         <v>596</v>
       </c>
-      <c r="D2" s="147" t="s">
+      <c r="D3" s="147" t="s">
         <v>600</v>
       </c>
-      <c r="E2" s="336" t="s">
+      <c r="E3" s="336" t="s">
         <v>595</v>
       </c>
-      <c r="F2" s="336" t="s">
+      <c r="F3" s="336" t="s">
         <v>596</v>
       </c>
-      <c r="G2" s="336" t="s">
+      <c r="G3" s="336" t="s">
         <v>600</v>
       </c>
-      <c r="H2" s="335" t="s">
+      <c r="H3" s="340" t="s">
+        <v>599</v>
+      </c>
+      <c r="I3" s="369" t="s">
+        <v>601</v>
+      </c>
+      <c r="J3" s="337" t="s">
+        <v>595</v>
+      </c>
+      <c r="K3" s="337" t="s">
+        <v>596</v>
+      </c>
+      <c r="L3" s="337" t="s">
+        <v>600</v>
+      </c>
+      <c r="M3" s="335" t="s">
         <v>598</v>
       </c>
-      <c r="I2" s="344" t="s">
-        <v>599</v>
-      </c>
-      <c r="J2" s="338" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" s="3" customFormat="1" ht="21" customHeight="1">
-      <c r="A3" s="374">
+    </row>
+    <row r="4" spans="1:13" s="3" customFormat="1" ht="21" customHeight="1">
+      <c r="A4" s="363">
         <v>18</v>
       </c>
-      <c r="B3" s="374" t="s">
+      <c r="B4" s="363" t="s">
         <v>219</v>
       </c>
-      <c r="C3" s="374" t="s">
+      <c r="C4" s="363" t="s">
         <v>219</v>
       </c>
-      <c r="D3" s="374" t="s">
+      <c r="D4" s="363" t="s">
         <v>219</v>
       </c>
-      <c r="E3" s="374" t="s">
+      <c r="E4" s="363" t="s">
         <v>219</v>
       </c>
-      <c r="F3" s="374" t="s">
+      <c r="F4" s="363" t="s">
         <v>219</v>
       </c>
-      <c r="G3" s="374" t="s">
+      <c r="G4" s="363" t="s">
         <v>219</v>
       </c>
-      <c r="H3" s="374" t="s">
+      <c r="H4" s="364"/>
+      <c r="I4" s="370" t="s">
+        <v>602</v>
+      </c>
+      <c r="M4" s="363" t="s">
         <v>219</v>
       </c>
-      <c r="I3" s="375"/>
-      <c r="J3" s="337" t="s">
+    </row>
+    <row r="5" spans="1:13" s="3" customFormat="1">
+      <c r="A5" s="363">
+        <v>10</v>
+      </c>
+      <c r="B5" s="363" t="s">
+        <v>219</v>
+      </c>
+      <c r="C5" s="363" t="s">
+        <v>219</v>
+      </c>
+      <c r="D5" s="363" t="s">
+        <v>219</v>
+      </c>
+      <c r="E5" s="363" t="s">
+        <v>219</v>
+      </c>
+      <c r="F5" s="363"/>
+      <c r="G5" s="363"/>
+      <c r="H5" s="364"/>
+      <c r="I5" s="370" t="s">
         <v>602</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" s="3" customFormat="1">
-      <c r="A4" s="374">
-        <v>10</v>
-      </c>
-      <c r="B4" s="374" t="s">
+      <c r="M5" s="363" t="s">
         <v>219</v>
       </c>
-      <c r="C4" s="374" t="s">
+    </row>
+    <row r="6" spans="1:13" s="3" customFormat="1">
+      <c r="A6" s="363">
+        <v>14</v>
+      </c>
+      <c r="B6" s="363" t="s">
         <v>219</v>
       </c>
-      <c r="D4" s="374" t="s">
+      <c r="C6" s="363" t="s">
         <v>219</v>
       </c>
-      <c r="E4" s="374" t="s">
+      <c r="D6" s="363"/>
+      <c r="E6" s="363" t="s">
         <v>219</v>
       </c>
-      <c r="F4" s="374"/>
-      <c r="G4" s="374"/>
-      <c r="H4" s="374" t="s">
+      <c r="F6" s="363"/>
+      <c r="G6" s="363"/>
+      <c r="H6" s="364"/>
+      <c r="I6" s="370" t="s">
+        <v>602</v>
+      </c>
+      <c r="M6" s="363" t="s">
         <v>219</v>
       </c>
-      <c r="I4" s="375"/>
-      <c r="J4" s="337" t="s">
+    </row>
+    <row r="7" spans="1:13" s="345" customFormat="1" ht="18" customHeight="1">
+      <c r="A7" s="343">
+        <v>3</v>
+      </c>
+      <c r="B7" s="343" t="s">
+        <v>219</v>
+      </c>
+      <c r="C7" s="343" t="s">
+        <v>219</v>
+      </c>
+      <c r="D7" s="343" t="s">
+        <v>219</v>
+      </c>
+      <c r="E7" s="343"/>
+      <c r="F7" s="343"/>
+      <c r="G7" s="343" t="s">
+        <v>219</v>
+      </c>
+      <c r="H7" s="344"/>
+      <c r="I7" s="371" t="s">
         <v>602</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" s="3" customFormat="1">
-      <c r="A5" s="374">
-        <v>14</v>
-      </c>
-      <c r="B5" s="374" t="s">
+      <c r="M7" s="343" t="s">
         <v>219</v>
       </c>
-      <c r="C5" s="374" t="s">
+    </row>
+    <row r="8" spans="1:13" s="345" customFormat="1" ht="18" customHeight="1">
+      <c r="A8" s="343">
+        <v>7</v>
+      </c>
+      <c r="B8" s="343" t="s">
         <v>219</v>
       </c>
-      <c r="D5" s="374"/>
-      <c r="E5" s="374" t="s">
+      <c r="C8" s="343" t="s">
         <v>219</v>
       </c>
-      <c r="F5" s="374"/>
-      <c r="G5" s="374"/>
-      <c r="H5" s="374" t="s">
+      <c r="D8" s="343" t="s">
         <v>219</v>
       </c>
-      <c r="I5" s="375"/>
-      <c r="J5" s="337" t="s">
+      <c r="E8" s="343"/>
+      <c r="F8" s="343"/>
+      <c r="G8" s="343" t="s">
+        <v>219</v>
+      </c>
+      <c r="H8" s="344"/>
+      <c r="I8" s="371" t="s">
         <v>602</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" s="350" customFormat="1" ht="18" customHeight="1">
-      <c r="A6" s="347">
-        <v>3</v>
-      </c>
-      <c r="B6" s="347" t="s">
+      <c r="M8" s="343" t="s">
         <v>219</v>
       </c>
-      <c r="C6" s="347" t="s">
+    </row>
+    <row r="9" spans="1:13" s="345" customFormat="1" ht="18" customHeight="1">
+      <c r="A9" s="343">
+        <v>8</v>
+      </c>
+      <c r="B9" s="343" t="s">
         <v>219</v>
       </c>
-      <c r="D6" s="347" t="s">
+      <c r="C9" s="343" t="s">
         <v>219</v>
       </c>
-      <c r="E6" s="347"/>
-      <c r="F6" s="347"/>
-      <c r="G6" s="347" t="s">
+      <c r="D9" s="343" t="s">
         <v>219</v>
       </c>
-      <c r="H6" s="347" t="s">
+      <c r="E9" s="343"/>
+      <c r="F9" s="343"/>
+      <c r="G9" s="343" t="s">
         <v>219</v>
       </c>
-      <c r="I6" s="348"/>
-      <c r="J6" s="349" t="s">
+      <c r="H9" s="344"/>
+      <c r="I9" s="371" t="s">
         <v>602</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" s="350" customFormat="1" ht="18" customHeight="1">
-      <c r="A7" s="347">
-        <v>7</v>
-      </c>
-      <c r="B7" s="347" t="s">
+      <c r="M9" s="343" t="s">
         <v>219</v>
       </c>
-      <c r="C7" s="347" t="s">
+    </row>
+    <row r="10" spans="1:13" s="30" customFormat="1" ht="16.5" customHeight="1">
+      <c r="A10" s="346">
+        <v>13</v>
+      </c>
+      <c r="B10" s="346" t="s">
         <v>219</v>
       </c>
-      <c r="D7" s="347" t="s">
+      <c r="C10" s="346" t="s">
         <v>219</v>
       </c>
-      <c r="E7" s="347"/>
-      <c r="F7" s="347"/>
-      <c r="G7" s="347" t="s">
+      <c r="D10" s="346"/>
+      <c r="E10" s="346"/>
+      <c r="F10" s="346"/>
+      <c r="G10" s="346" t="s">
         <v>219</v>
       </c>
-      <c r="H7" s="347" t="s">
+      <c r="H10" s="347"/>
+      <c r="I10" s="372" t="s">
+        <v>602</v>
+      </c>
+      <c r="M10" s="346" t="s">
         <v>219</v>
       </c>
-      <c r="I7" s="348"/>
-      <c r="J7" s="349" t="s">
+    </row>
+    <row r="11" spans="1:13" s="30" customFormat="1">
+      <c r="A11" s="346">
+        <v>15</v>
+      </c>
+      <c r="B11" s="346" t="s">
+        <v>219</v>
+      </c>
+      <c r="C11" s="346" t="s">
+        <v>219</v>
+      </c>
+      <c r="D11" s="346"/>
+      <c r="E11" s="346"/>
+      <c r="F11" s="346"/>
+      <c r="G11" s="346" t="s">
+        <v>219</v>
+      </c>
+      <c r="H11" s="347"/>
+      <c r="I11" s="372" t="s">
         <v>602</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" s="350" customFormat="1" ht="18" customHeight="1">
-      <c r="A8" s="347">
-        <v>8</v>
-      </c>
-      <c r="B8" s="347" t="s">
+      <c r="M11" s="346" t="s">
         <v>219</v>
       </c>
-      <c r="C8" s="347" t="s">
+    </row>
+    <row r="12" spans="1:13" s="345" customFormat="1">
+      <c r="A12" s="343">
+        <v>17</v>
+      </c>
+      <c r="B12" s="343" t="s">
         <v>219</v>
       </c>
-      <c r="D8" s="347" t="s">
+      <c r="C12" s="343" t="s">
         <v>219</v>
       </c>
-      <c r="E8" s="347"/>
-      <c r="F8" s="347"/>
-      <c r="G8" s="347" t="s">
+      <c r="D12" s="343" t="s">
         <v>219</v>
       </c>
-      <c r="H8" s="347" t="s">
+      <c r="E12" s="343"/>
+      <c r="F12" s="343"/>
+      <c r="G12" s="343" t="s">
         <v>219</v>
       </c>
-      <c r="I8" s="348"/>
-      <c r="J8" s="349" t="s">
+      <c r="H12" s="344"/>
+      <c r="I12" s="371" t="s">
         <v>602</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" s="30" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A9" s="351">
-        <v>13</v>
-      </c>
-      <c r="B9" s="351" t="s">
+      <c r="M12" s="343" t="s">
         <v>219</v>
       </c>
-      <c r="C9" s="351" t="s">
+    </row>
+    <row r="13" spans="1:13" s="3" customFormat="1">
+      <c r="A13" s="363">
+        <v>1</v>
+      </c>
+      <c r="B13" s="363" t="s">
         <v>219</v>
       </c>
-      <c r="D9" s="351"/>
-      <c r="E9" s="351"/>
-      <c r="F9" s="351"/>
-      <c r="G9" s="351" t="s">
+      <c r="C13" s="363"/>
+      <c r="D13" s="363"/>
+      <c r="E13" s="363"/>
+      <c r="F13" s="363"/>
+      <c r="G13" s="363"/>
+      <c r="H13" s="364"/>
+      <c r="I13" s="370" t="s">
+        <v>602</v>
+      </c>
+      <c r="M13" s="363" t="s">
         <v>219</v>
       </c>
-      <c r="H9" s="351" t="s">
+    </row>
+    <row r="14" spans="1:13" s="3" customFormat="1">
+      <c r="A14" s="363">
+        <v>5</v>
+      </c>
+      <c r="B14" s="363" t="s">
         <v>219</v>
       </c>
-      <c r="I9" s="352"/>
-      <c r="J9" s="353" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" s="30" customFormat="1">
-      <c r="A10" s="351">
-        <v>15</v>
-      </c>
-      <c r="B10" s="351" t="s">
+      <c r="C14" s="363" t="s">
         <v>219</v>
       </c>
-      <c r="C10" s="351" t="s">
+      <c r="D14" s="363" t="s">
         <v>219</v>
       </c>
-      <c r="D10" s="351"/>
-      <c r="E10" s="351"/>
-      <c r="F10" s="351"/>
-      <c r="G10" s="351" t="s">
+      <c r="E14" s="363"/>
+      <c r="F14" s="363"/>
+      <c r="G14" s="363"/>
+      <c r="H14" s="364" t="s">
         <v>219</v>
       </c>
-      <c r="H10" s="351" t="s">
+      <c r="I14" s="370" t="s">
+        <v>603</v>
+      </c>
+      <c r="M14" s="363" t="s">
         <v>219</v>
       </c>
-      <c r="I10" s="352"/>
-      <c r="J10" s="353" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" s="350" customFormat="1">
-      <c r="A11" s="347">
-        <v>17</v>
-      </c>
-      <c r="B11" s="347" t="s">
+    </row>
+    <row r="15" spans="1:13" s="359" customFormat="1">
+      <c r="A15" s="357">
+        <v>2</v>
+      </c>
+      <c r="B15" s="357" t="s">
         <v>219</v>
       </c>
-      <c r="C11" s="347" t="s">
+      <c r="C15" s="357"/>
+      <c r="D15" s="357" t="s">
         <v>219</v>
       </c>
-      <c r="D11" s="347" t="s">
+      <c r="E15" s="357"/>
+      <c r="F15" s="357"/>
+      <c r="G15" s="357" t="s">
         <v>219</v>
       </c>
-      <c r="E11" s="347"/>
-      <c r="F11" s="347"/>
-      <c r="G11" s="347" t="s">
+      <c r="H15" s="358"/>
+      <c r="I15" s="373" t="s">
+        <v>604</v>
+      </c>
+      <c r="M15" s="357"/>
+    </row>
+    <row r="16" spans="1:13" s="359" customFormat="1">
+      <c r="A16" s="357">
+        <v>4</v>
+      </c>
+      <c r="B16" s="357" t="s">
         <v>219</v>
       </c>
-      <c r="H11" s="347" t="s">
+      <c r="C16" s="357"/>
+      <c r="D16" s="357" t="s">
         <v>219</v>
       </c>
-      <c r="I11" s="348"/>
-      <c r="J11" s="349" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" s="3" customFormat="1">
-      <c r="A12" s="374">
-        <v>1</v>
-      </c>
-      <c r="B12" s="374" t="s">
+      <c r="E16" s="357"/>
+      <c r="F16" s="357"/>
+      <c r="G16" s="357" t="s">
         <v>219</v>
       </c>
-      <c r="C12" s="374"/>
-      <c r="D12" s="374"/>
-      <c r="E12" s="374"/>
-      <c r="F12" s="374"/>
-      <c r="G12" s="374"/>
-      <c r="H12" s="374" t="s">
+      <c r="H16" s="358"/>
+      <c r="I16" s="373" t="s">
+        <v>604</v>
+      </c>
+      <c r="M16" s="357"/>
+    </row>
+    <row r="17" spans="1:13" s="362" customFormat="1">
+      <c r="A17" s="360">
+        <v>6</v>
+      </c>
+      <c r="B17" s="360" t="s">
         <v>219</v>
       </c>
-      <c r="I12" s="375"/>
-      <c r="J12" s="337" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" s="3" customFormat="1">
-      <c r="A13" s="374">
-        <v>5</v>
-      </c>
-      <c r="B13" s="374" t="s">
+      <c r="C17" s="360" t="s">
         <v>219</v>
       </c>
-      <c r="C13" s="374" t="s">
+      <c r="D17" s="360"/>
+      <c r="E17" s="360"/>
+      <c r="F17" s="360"/>
+      <c r="G17" s="360" t="s">
         <v>219</v>
       </c>
-      <c r="D13" s="374" t="s">
+      <c r="H17" s="361"/>
+      <c r="I17" s="374" t="s">
+        <v>604</v>
+      </c>
+      <c r="M17" s="360"/>
+    </row>
+    <row r="18" spans="1:13" s="362" customFormat="1">
+      <c r="A18" s="360">
+        <v>11</v>
+      </c>
+      <c r="B18" s="360" t="s">
         <v>219</v>
       </c>
-      <c r="E13" s="374"/>
-      <c r="F13" s="374"/>
-      <c r="G13" s="374"/>
-      <c r="H13" s="374" t="s">
+      <c r="C18" s="360" t="s">
         <v>219</v>
       </c>
-      <c r="I13" s="375" t="s">
+      <c r="D18" s="360"/>
+      <c r="E18" s="360"/>
+      <c r="F18" s="360"/>
+      <c r="G18" s="360" t="s">
         <v>219</v>
       </c>
-      <c r="J13" s="376" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" s="369" customFormat="1">
-      <c r="A14" s="366">
-        <v>2</v>
-      </c>
-      <c r="B14" s="366" t="s">
+      <c r="H18" s="361"/>
+      <c r="I18" s="374" t="s">
+        <v>605</v>
+      </c>
+      <c r="M18" s="360"/>
+    </row>
+    <row r="19" spans="1:13" s="3" customFormat="1">
+      <c r="A19" s="363">
+        <v>19</v>
+      </c>
+      <c r="B19" s="363" t="s">
         <v>219</v>
       </c>
-      <c r="C14" s="366"/>
-      <c r="D14" s="366" t="s">
+      <c r="C19" s="363"/>
+      <c r="D19" s="363" t="s">
         <v>219</v>
       </c>
-      <c r="E14" s="366"/>
-      <c r="F14" s="366"/>
-      <c r="G14" s="366" t="s">
+      <c r="E19" s="363"/>
+      <c r="F19" s="363"/>
+      <c r="G19" s="363" t="s">
         <v>219</v>
       </c>
-      <c r="H14" s="366"/>
-      <c r="I14" s="367"/>
-      <c r="J14" s="368" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" s="369" customFormat="1">
-      <c r="A15" s="366">
-        <v>4</v>
-      </c>
-      <c r="B15" s="366" t="s">
+      <c r="H19" s="364" t="s">
         <v>219</v>
       </c>
-      <c r="C15" s="366"/>
-      <c r="D15" s="366" t="s">
+      <c r="I19" s="370" t="s">
+        <v>606</v>
+      </c>
+      <c r="M19" s="363"/>
+    </row>
+    <row r="20" spans="1:13" s="350" customFormat="1">
+      <c r="A20" s="348">
+        <v>20</v>
+      </c>
+      <c r="B20" s="348" t="s">
         <v>219</v>
       </c>
-      <c r="E15" s="366"/>
-      <c r="F15" s="366"/>
-      <c r="G15" s="366" t="s">
+      <c r="C20" s="348"/>
+      <c r="D20" s="348"/>
+      <c r="E20" s="348"/>
+      <c r="F20" s="348"/>
+      <c r="G20" s="348" t="s">
         <v>219</v>
       </c>
-      <c r="H15" s="366"/>
-      <c r="I15" s="367"/>
-      <c r="J15" s="368" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" s="373" customFormat="1">
-      <c r="A16" s="370">
-        <v>6</v>
-      </c>
-      <c r="B16" s="370" t="s">
+      <c r="H20" s="349" t="s">
         <v>219</v>
       </c>
-      <c r="C16" s="370" t="s">
+      <c r="I20" s="375" t="s">
+        <v>606</v>
+      </c>
+      <c r="M20" s="348"/>
+    </row>
+    <row r="21" spans="1:13" s="350" customFormat="1">
+      <c r="A21" s="348">
+        <v>21</v>
+      </c>
+      <c r="B21" s="348" t="s">
         <v>219</v>
       </c>
-      <c r="D16" s="370"/>
-      <c r="E16" s="370"/>
-      <c r="F16" s="370"/>
-      <c r="G16" s="370" t="s">
+      <c r="C21" s="348"/>
+      <c r="D21" s="348"/>
+      <c r="E21" s="348"/>
+      <c r="F21" s="348"/>
+      <c r="G21" s="348" t="s">
         <v>219</v>
       </c>
-      <c r="H16" s="370"/>
-      <c r="I16" s="371"/>
-      <c r="J16" s="372" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" s="373" customFormat="1">
-      <c r="A17" s="370">
-        <v>11</v>
-      </c>
-      <c r="B17" s="370" t="s">
+      <c r="H21" s="349" t="s">
         <v>219</v>
       </c>
-      <c r="C17" s="370" t="s">
+      <c r="I21" s="375" t="s">
+        <v>606</v>
+      </c>
+      <c r="M21" s="348"/>
+    </row>
+    <row r="22" spans="1:13" s="353" customFormat="1">
+      <c r="A22" s="351">
+        <v>9</v>
+      </c>
+      <c r="B22" s="351" t="s">
         <v>219</v>
       </c>
-      <c r="D17" s="370"/>
-      <c r="E17" s="370"/>
-      <c r="F17" s="370"/>
-      <c r="G17" s="370" t="s">
+      <c r="C22" s="351" t="s">
         <v>219</v>
       </c>
-      <c r="H17" s="370"/>
-      <c r="I17" s="371"/>
-      <c r="J17" s="372" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" s="3" customFormat="1">
-      <c r="A18" s="374">
-        <v>19</v>
-      </c>
-      <c r="B18" s="374" t="s">
+      <c r="D22" s="351"/>
+      <c r="E22" s="351"/>
+      <c r="F22" s="351"/>
+      <c r="G22" s="351"/>
+      <c r="H22" s="352"/>
+      <c r="I22" s="376" t="s">
+        <v>607</v>
+      </c>
+      <c r="M22" s="351"/>
+    </row>
+    <row r="23" spans="1:13" s="356" customFormat="1" ht="33" customHeight="1">
+      <c r="A23" s="354">
+        <v>12</v>
+      </c>
+      <c r="B23" s="354" t="s">
         <v>219</v>
       </c>
-      <c r="C18" s="374"/>
-      <c r="D18" s="374" t="s">
+      <c r="C23" s="354" t="s">
         <v>219</v>
       </c>
-      <c r="E18" s="374"/>
-      <c r="F18" s="374"/>
-      <c r="G18" s="374" t="s">
+      <c r="D23" s="354" t="s">
         <v>219</v>
       </c>
-      <c r="H18" s="374"/>
-      <c r="I18" s="375" t="s">
+      <c r="E23" s="354"/>
+      <c r="F23" s="354"/>
+      <c r="G23" s="354"/>
+      <c r="H23" s="355"/>
+      <c r="I23" s="377" t="s">
+        <v>607</v>
+      </c>
+      <c r="M23" s="354"/>
+    </row>
+    <row r="24" spans="1:13" s="356" customFormat="1">
+      <c r="A24" s="354">
+        <v>16</v>
+      </c>
+      <c r="B24" s="354" t="s">
         <v>219</v>
       </c>
-      <c r="J18" s="376" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" s="357" customFormat="1">
-      <c r="A19" s="354">
-        <v>20</v>
-      </c>
-      <c r="B19" s="354" t="s">
+      <c r="C24" s="354" t="s">
         <v>219</v>
       </c>
-      <c r="C19" s="354"/>
-      <c r="D19" s="354"/>
-      <c r="E19" s="354"/>
-      <c r="F19" s="354"/>
-      <c r="G19" s="354" t="s">
+      <c r="D24" s="354" t="s">
         <v>219</v>
       </c>
-      <c r="H19" s="354"/>
-      <c r="I19" s="355" t="s">
+      <c r="E24" s="354"/>
+      <c r="F24" s="354"/>
+      <c r="G24" s="354"/>
+      <c r="H24" s="355"/>
+      <c r="I24" s="377" t="s">
+        <v>607</v>
+      </c>
+      <c r="M24" s="354"/>
+    </row>
+    <row r="25" spans="1:13" s="353" customFormat="1">
+      <c r="A25" s="351">
+        <v>22</v>
+      </c>
+      <c r="B25" s="351" t="s">
         <v>219</v>
       </c>
-      <c r="J19" s="356" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" s="357" customFormat="1">
-      <c r="A20" s="354">
-        <v>21</v>
-      </c>
-      <c r="B20" s="354" t="s">
+      <c r="C25" s="351" t="s">
         <v>219</v>
       </c>
-      <c r="C20" s="354"/>
-      <c r="D20" s="354"/>
-      <c r="E20" s="354"/>
-      <c r="F20" s="354"/>
-      <c r="G20" s="354" t="s">
-        <v>219</v>
-      </c>
-      <c r="H20" s="354"/>
-      <c r="I20" s="355" t="s">
-        <v>219</v>
-      </c>
-      <c r="J20" s="356" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" s="361" customFormat="1">
-      <c r="A21" s="358">
-        <v>9</v>
-      </c>
-      <c r="B21" s="358" t="s">
-        <v>219</v>
-      </c>
-      <c r="C21" s="358" t="s">
-        <v>219</v>
-      </c>
-      <c r="D21" s="358"/>
-      <c r="E21" s="358"/>
-      <c r="F21" s="358"/>
-      <c r="G21" s="358"/>
-      <c r="H21" s="358"/>
-      <c r="I21" s="359"/>
-      <c r="J21" s="360" t="s">
+      <c r="D25" s="351"/>
+      <c r="E25" s="351"/>
+      <c r="F25" s="351"/>
+      <c r="G25" s="351"/>
+      <c r="H25" s="352"/>
+      <c r="I25" s="376" t="s">
         <v>607</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" s="365" customFormat="1" ht="33" customHeight="1">
-      <c r="A22" s="362">
-        <v>12</v>
-      </c>
-      <c r="B22" s="362" t="s">
-        <v>219</v>
-      </c>
-      <c r="C22" s="362" t="s">
-        <v>219</v>
-      </c>
-      <c r="D22" s="362" t="s">
-        <v>219</v>
-      </c>
-      <c r="E22" s="362"/>
-      <c r="F22" s="362"/>
-      <c r="G22" s="362"/>
-      <c r="H22" s="362"/>
-      <c r="I22" s="363"/>
-      <c r="J22" s="364" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" s="365" customFormat="1">
-      <c r="A23" s="362">
-        <v>16</v>
-      </c>
-      <c r="B23" s="362" t="s">
-        <v>219</v>
-      </c>
-      <c r="C23" s="362" t="s">
-        <v>219</v>
-      </c>
-      <c r="D23" s="362" t="s">
-        <v>219</v>
-      </c>
-      <c r="E23" s="362"/>
-      <c r="F23" s="362"/>
-      <c r="G23" s="362"/>
-      <c r="H23" s="362"/>
-      <c r="I23" s="363"/>
-      <c r="J23" s="364" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" s="361" customFormat="1">
-      <c r="A24" s="358">
-        <v>22</v>
-      </c>
-      <c r="B24" s="358" t="s">
-        <v>219</v>
-      </c>
-      <c r="C24" s="358" t="s">
-        <v>219</v>
-      </c>
-      <c r="D24" s="358"/>
-      <c r="E24" s="358"/>
-      <c r="F24" s="358"/>
-      <c r="G24" s="358"/>
-      <c r="H24" s="358"/>
-      <c r="I24" s="359"/>
-      <c r="J24" s="360" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11">
-      <c r="J25" s="320"/>
-    </row>
-    <row r="26" spans="1:11">
-      <c r="I26" s="346"/>
-      <c r="J26" s="320"/>
-      <c r="K26" s="320"/>
-    </row>
-    <row r="27" spans="1:11">
-      <c r="I27" s="346"/>
+      <c r="M25" s="351"/>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="I26" s="378"/>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="H27" s="342"/>
+      <c r="I27" s="378"/>
       <c r="J27" s="320"/>
-      <c r="K27" s="320"/>
-    </row>
-    <row r="28" spans="1:11">
-      <c r="I28" s="346"/>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="H28" s="342"/>
+      <c r="I28" s="378"/>
       <c r="J28" s="320"/>
-      <c r="K28" s="320"/>
-    </row>
-    <row r="29" spans="1:11">
-      <c r="I29" s="346"/>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="H29" s="342"/>
+      <c r="I29" s="378"/>
       <c r="J29" s="320"/>
-      <c r="K29" s="320"/>
-    </row>
-    <row r="30" spans="1:11">
-      <c r="I30" s="346"/>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="H30" s="342"/>
+      <c r="I30" s="378"/>
       <c r="J30" s="320"/>
-      <c r="K30" s="320"/>
-    </row>
-    <row r="31" spans="1:11">
-      <c r="I31" s="346"/>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="H31" s="342"/>
+      <c r="I31" s="378"/>
       <c r="J31" s="320"/>
-      <c r="K31" s="320"/>
-    </row>
-    <row r="32" spans="1:11">
-      <c r="I32" s="346"/>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="H32" s="342"/>
+      <c r="I32" s="378"/>
       <c r="J32" s="320"/>
-      <c r="K32" s="320"/>
-    </row>
-    <row r="33" spans="9:11">
-      <c r="I33" s="346"/>
+    </row>
+    <row r="33" spans="8:10">
+      <c r="H33" s="342"/>
+      <c r="I33" s="378"/>
       <c r="J33" s="320"/>
-      <c r="K33" s="320"/>
-    </row>
-    <row r="34" spans="9:11">
-      <c r="I34" s="346"/>
+    </row>
+    <row r="34" spans="8:10">
+      <c r="H34" s="342"/>
+      <c r="I34" s="378"/>
       <c r="J34" s="320"/>
-      <c r="K34" s="320"/>
-    </row>
-    <row r="35" spans="9:11">
-      <c r="I35" s="346"/>
+    </row>
+    <row r="35" spans="8:10">
+      <c r="H35" s="342"/>
+      <c r="I35" s="378"/>
       <c r="J35" s="320"/>
-      <c r="K35" s="320"/>
-    </row>
-    <row r="36" spans="9:11">
-      <c r="I36" s="346"/>
+    </row>
+    <row r="36" spans="8:10">
+      <c r="H36" s="342"/>
+      <c r="I36" s="378"/>
       <c r="J36" s="320"/>
-      <c r="K36" s="320"/>
-    </row>
-    <row r="37" spans="9:11">
-      <c r="I37" s="346"/>
+    </row>
+    <row r="37" spans="8:10">
+      <c r="H37" s="342"/>
+      <c r="I37" s="378"/>
       <c r="J37" s="320"/>
-      <c r="K37" s="320"/>
-    </row>
-    <row r="38" spans="9:11">
-      <c r="I38" s="346"/>
+    </row>
+    <row r="38" spans="8:10">
+      <c r="H38" s="342"/>
+      <c r="I38" s="378"/>
       <c r="J38" s="320"/>
-      <c r="K38" s="320"/>
-    </row>
-    <row r="39" spans="9:11">
-      <c r="I39" s="346"/>
+    </row>
+    <row r="39" spans="8:10">
+      <c r="H39" s="342"/>
+      <c r="I39" s="378"/>
       <c r="J39" s="320"/>
-      <c r="K39" s="320"/>
-    </row>
-    <row r="40" spans="9:11">
-      <c r="I40" s="346"/>
+    </row>
+    <row r="40" spans="8:10">
+      <c r="H40" s="342"/>
+      <c r="I40" s="378"/>
       <c r="J40" s="320"/>
-      <c r="K40" s="320"/>
-    </row>
-    <row r="41" spans="9:11">
-      <c r="I41" s="346"/>
+    </row>
+    <row r="41" spans="8:10">
+      <c r="H41" s="342"/>
+      <c r="I41" s="378"/>
       <c r="J41" s="320"/>
-      <c r="K41" s="320"/>
+    </row>
+    <row r="42" spans="8:10">
+      <c r="H42" s="342"/>
+      <c r="I42" s="378"/>
+      <c r="J42" s="320"/>
     </row>
   </sheetData>
   <sortState ref="A3:I24">
-    <sortCondition ref="H3:H24"/>
     <sortCondition ref="E3:E24"/>
     <sortCondition ref="F3:F24"/>
     <sortCondition ref="G3:G24"/>
   </sortState>
-  <mergeCells count="2">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
+  <mergeCells count="3">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="J2:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>